<commit_message>
Fix Hb export in India
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_india.xlsx
+++ b/inst/extdata/main_dict_india.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1451,9 +1451,6 @@
     <t>crfs-t08a-f2_4</t>
   </si>
   <si>
-    <t>crfs-t08a-f2_5</t>
-  </si>
-  <si>
     <t>crfs-t08a-f2_10a</t>
   </si>
   <si>
@@ -1956,6 +1953,9 @@
   </si>
   <si>
     <t>instanceID</t>
+  </si>
+  <si>
+    <t>crfs-t08a-f2_5a</t>
   </si>
 </sst>
 </file>
@@ -2381,22 +2381,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="A222" sqref="A222:XFD222"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
     <col min="5" max="5" width="9.25" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="3"/>
-    <col min="8" max="8" width="31.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2416,13 +2416,13 @@
         <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -2500,9 +2500,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>172</v>
@@ -2523,16 +2523,16 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>640</v>
-      </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -2549,15 +2549,15 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2575,68 +2575,68 @@
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>613</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>613</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>638</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>638</v>
-      </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
@@ -2653,166 +2653,166 @@
         <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>620</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
         <v>621</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="B12" s="24" t="s">
         <v>622</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>623</v>
       </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="B13" s="24" t="s">
         <v>624</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
         <v>625</v>
       </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="B14" s="24" t="s">
         <v>626</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
         <v>627</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="B15" s="19" t="s">
         <v>628</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
         <v>629</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="19" t="s">
+      <c r="B16" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
-        <v>630</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>631</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>333</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>334</v>
       </c>
@@ -2864,12 +2864,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -2887,10 +2887,10 @@
         <v>0</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>335</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>336</v>
       </c>
@@ -2942,33 +2942,33 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>497</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>337</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>338</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>339</v>
       </c>
@@ -3046,12 +3046,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -3069,10 +3069,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>341</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>342</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>343</v>
       </c>
@@ -3150,12 +3150,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>340</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -3176,7 +3176,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>344</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>345</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>346</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>347</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>348</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>349</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>350</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>351</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>352</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>353</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>354</v>
       </c>
@@ -3462,59 +3462,59 @@
         <v>192</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>507</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1</v>
+      </c>
+      <c r="H42" s="12" t="s">
         <v>508</v>
       </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2">
-        <v>0</v>
-      </c>
-      <c r="E42" s="4">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3">
-        <v>1</v>
-      </c>
-      <c r="H42" s="12" t="s">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="12" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
-        <v>511</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>512</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2">
-        <v>0</v>
-      </c>
-      <c r="E43" s="4">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3">
-        <v>0</v>
-      </c>
-      <c r="G43" s="3">
-        <v>0</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>355</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>356</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>357</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>358</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>359</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>360</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>361</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>362</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>363</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>364</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>365</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>366</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>367</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>369</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>370</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>368</v>
       </c>
@@ -3930,9 +3930,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>32</v>
@@ -3956,9 +3956,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>33</v>
@@ -3982,35 +3982,35 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B62" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="4">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>1</v>
+      </c>
+      <c r="H62" s="11" t="s">
         <v>561</v>
       </c>
-      <c r="C62" s="2">
-        <v>0</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="4">
-        <v>1</v>
-      </c>
-      <c r="F62" s="3">
-        <v>0</v>
-      </c>
-      <c r="G62" s="3">
-        <v>1</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>38</v>
@@ -4034,9 +4034,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>39</v>
@@ -4060,38 +4060,38 @@
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>634</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="C65" s="2">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="4">
+        <v>0</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="C65" s="2">
-        <v>0</v>
-      </c>
-      <c r="D65" s="2">
-        <v>1</v>
-      </c>
-      <c r="E65" s="4">
-        <v>0</v>
-      </c>
-      <c r="F65" s="4">
-        <v>0</v>
-      </c>
-      <c r="G65" s="3">
-        <v>0</v>
-      </c>
-      <c r="H65" s="9" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
@@ -4109,36 +4109,36 @@
         <v>0</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="B67" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="C67" s="2">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="4">
+        <v>0</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0</v>
+      </c>
+      <c r="H67" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="C67" s="2">
-        <v>0</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
-      </c>
-      <c r="E67" s="4">
-        <v>0</v>
-      </c>
-      <c r="F67" s="4">
-        <v>0</v>
-      </c>
-      <c r="G67" s="3">
-        <v>0</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>371</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>372</v>
       </c>
@@ -4190,39 +4190,39 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="B70" s="19" t="s">
+      <c r="C70" s="2">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+      <c r="E70" s="4">
+        <v>1</v>
+      </c>
+      <c r="F70" s="4">
+        <v>1</v>
+      </c>
+      <c r="G70" s="3">
+        <v>1</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1</v>
-      </c>
-      <c r="E70" s="4">
-        <v>1</v>
-      </c>
-      <c r="F70" s="4">
-        <v>1</v>
-      </c>
-      <c r="G70" s="3">
-        <v>1</v>
-      </c>
-      <c r="H70" s="11" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="19" t="s">
+      <c r="B71" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="B71" s="19" t="s">
-        <v>506</v>
-      </c>
       <c r="C71" s="2">
         <v>1</v>
       </c>
@@ -4239,15 +4239,15 @@
         <v>1</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -4265,88 +4265,88 @@
         <v>1</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="B73" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="4">
+        <v>1</v>
+      </c>
+      <c r="F73" s="4">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3">
+        <v>1</v>
+      </c>
+      <c r="H73" s="11" t="s">
         <v>553</v>
       </c>
-      <c r="C73" s="2">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2">
-        <v>1</v>
-      </c>
-      <c r="E73" s="4">
-        <v>1</v>
-      </c>
-      <c r="F73" s="4">
-        <v>0</v>
-      </c>
-      <c r="G73" s="3">
-        <v>1</v>
-      </c>
-      <c r="H73" s="11" t="s">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="11" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="11" t="s">
+      <c r="B74" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="4">
+        <v>1</v>
+      </c>
+      <c r="F74" s="4">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3">
+        <v>1</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
         <v>555</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B75" s="11" t="s">
         <v>557</v>
       </c>
-      <c r="C74" s="2">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2">
-        <v>1</v>
-      </c>
-      <c r="E74" s="4">
-        <v>1</v>
-      </c>
-      <c r="F74" s="4">
-        <v>0</v>
-      </c>
-      <c r="G74" s="3">
-        <v>1</v>
-      </c>
-      <c r="H74" s="11" t="s">
+      <c r="C75" s="2">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="4">
+        <v>1</v>
+      </c>
+      <c r="F75" s="4">
+        <v>0</v>
+      </c>
+      <c r="G75" s="3">
+        <v>1</v>
+      </c>
+      <c r="H75" s="11" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
-        <v>556</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="C75" s="2">
-        <v>1</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="4">
-        <v>1</v>
-      </c>
-      <c r="F75" s="4">
-        <v>0</v>
-      </c>
-      <c r="G75" s="3">
-        <v>1</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
         <v>373</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
         <v>374</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
         <v>375</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
         <v>376</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
         <v>377</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
         <v>378</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
         <v>379</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
         <v>380</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
         <v>381</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>382</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>383</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>384</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>385</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>386</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
         <v>387</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
         <v>388</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
         <v>389</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
         <v>390</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
         <v>391</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
         <v>392</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
         <v>393</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
         <v>394</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
         <v>395</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
         <v>396</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
         <v>397</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
         <v>398</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
         <v>399</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
         <v>400</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
         <v>401</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
         <v>402</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
         <v>403</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
         <v>404</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
         <v>405</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
         <v>406</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
         <v>407</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
         <v>408</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
         <v>409</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
         <v>410</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
         <v>411</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
         <v>412</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
         <v>413</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
         <v>414</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
         <v>415</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
         <v>416</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
         <v>417</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
         <v>418</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
         <v>419</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
         <v>420</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
         <v>421</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
         <v>422</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
         <v>423</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
         <v>424</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
         <v>425</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
         <v>426</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
         <v>427</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
         <v>428</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
         <v>429</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
         <v>430</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
         <v>431</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
         <v>432</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
         <v>433</v>
       </c>
@@ -5932,7 +5932,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
         <v>434</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="17" t="s">
         <v>435</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="17" t="s">
         <v>436</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
         <v>437</v>
       </c>
@@ -6036,9 +6036,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B141" s="14" t="s">
         <v>116</v>
@@ -6059,10 +6059,10 @@
         <v>0</v>
       </c>
       <c r="H141" s="17" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
         <v>438</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
         <v>439</v>
       </c>
@@ -6114,33 +6114,33 @@
         <v>282</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B144" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="C144" s="2">
+        <v>0</v>
+      </c>
+      <c r="D144" s="2">
+        <v>0</v>
+      </c>
+      <c r="E144" s="20">
+        <v>1</v>
+      </c>
+      <c r="F144" s="22">
+        <v>1</v>
+      </c>
+      <c r="G144" s="3">
+        <v>0</v>
+      </c>
+      <c r="H144" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="C144" s="2">
-        <v>0</v>
-      </c>
-      <c r="D144" s="2">
-        <v>0</v>
-      </c>
-      <c r="E144" s="20">
-        <v>1</v>
-      </c>
-      <c r="F144" s="22">
-        <v>1</v>
-      </c>
-      <c r="G144" s="3">
-        <v>0</v>
-      </c>
-      <c r="H144" s="17" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
         <v>440</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
         <v>441</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
         <v>442</v>
       </c>
@@ -6218,165 +6218,165 @@
         <v>285</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="18" t="s">
+        <v>587</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="C148" s="2">
+        <v>0</v>
+      </c>
+      <c r="D148" s="2">
+        <v>0</v>
+      </c>
+      <c r="E148" s="20">
+        <v>1</v>
+      </c>
+      <c r="F148" s="20">
+        <v>1</v>
+      </c>
+      <c r="G148" s="3">
+        <v>0</v>
+      </c>
+      <c r="H148" s="18" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="18" t="s">
         <v>588</v>
       </c>
-      <c r="B148" s="16" t="s">
+      <c r="B149" s="16" t="s">
         <v>594</v>
       </c>
-      <c r="C148" s="2">
-        <v>0</v>
-      </c>
-      <c r="D148" s="2">
-        <v>0</v>
-      </c>
-      <c r="E148" s="20">
-        <v>1</v>
-      </c>
-      <c r="F148" s="20">
-        <v>1</v>
-      </c>
-      <c r="G148" s="3">
-        <v>0</v>
-      </c>
-      <c r="H148" s="18" t="s">
+      <c r="C149" s="2">
+        <v>0</v>
+      </c>
+      <c r="D149" s="2">
+        <v>0</v>
+      </c>
+      <c r="E149" s="20">
+        <v>1</v>
+      </c>
+      <c r="F149" s="20">
+        <v>1</v>
+      </c>
+      <c r="G149" s="3">
+        <v>0</v>
+      </c>
+      <c r="H149" s="18" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A149" s="18" t="s">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="18" t="s">
         <v>589</v>
       </c>
-      <c r="B149" s="16" t="s">
+      <c r="B150" s="16" t="s">
         <v>595</v>
       </c>
-      <c r="C149" s="2">
-        <v>0</v>
-      </c>
-      <c r="D149" s="2">
-        <v>0</v>
-      </c>
-      <c r="E149" s="20">
-        <v>1</v>
-      </c>
-      <c r="F149" s="20">
-        <v>1</v>
-      </c>
-      <c r="G149" s="3">
-        <v>0</v>
-      </c>
-      <c r="H149" s="18" t="s">
+      <c r="C150" s="2">
+        <v>0</v>
+      </c>
+      <c r="D150" s="2">
+        <v>0</v>
+      </c>
+      <c r="E150" s="20">
+        <v>1</v>
+      </c>
+      <c r="F150" s="20">
+        <v>1</v>
+      </c>
+      <c r="G150" s="3">
+        <v>0</v>
+      </c>
+      <c r="H150" s="18" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A150" s="18" t="s">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="18" t="s">
         <v>590</v>
       </c>
-      <c r="B150" s="16" t="s">
+      <c r="B151" s="16" t="s">
         <v>596</v>
       </c>
-      <c r="C150" s="2">
-        <v>0</v>
-      </c>
-      <c r="D150" s="2">
-        <v>0</v>
-      </c>
-      <c r="E150" s="20">
-        <v>1</v>
-      </c>
-      <c r="F150" s="20">
-        <v>1</v>
-      </c>
-      <c r="G150" s="3">
-        <v>0</v>
-      </c>
-      <c r="H150" s="18" t="s">
+      <c r="C151" s="2">
+        <v>0</v>
+      </c>
+      <c r="D151" s="2">
+        <v>0</v>
+      </c>
+      <c r="E151" s="20">
+        <v>1</v>
+      </c>
+      <c r="F151" s="20">
+        <v>1</v>
+      </c>
+      <c r="G151" s="3">
+        <v>0</v>
+      </c>
+      <c r="H151" s="18" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A151" s="18" t="s">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="18" t="s">
         <v>591</v>
       </c>
-      <c r="B151" s="16" t="s">
+      <c r="B152" s="16" t="s">
         <v>597</v>
       </c>
-      <c r="C151" s="2">
-        <v>0</v>
-      </c>
-      <c r="D151" s="2">
-        <v>0</v>
-      </c>
-      <c r="E151" s="20">
-        <v>1</v>
-      </c>
-      <c r="F151" s="20">
-        <v>1</v>
-      </c>
-      <c r="G151" s="3">
-        <v>0</v>
-      </c>
-      <c r="H151" s="18" t="s">
+      <c r="C152" s="2">
+        <v>0</v>
+      </c>
+      <c r="D152" s="2">
+        <v>0</v>
+      </c>
+      <c r="E152" s="20">
+        <v>1</v>
+      </c>
+      <c r="F152" s="20">
+        <v>1</v>
+      </c>
+      <c r="G152" s="3">
+        <v>0</v>
+      </c>
+      <c r="H152" s="18" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="18" t="s">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="18" t="s">
         <v>592</v>
       </c>
-      <c r="B152" s="16" t="s">
+      <c r="B153" s="16" t="s">
         <v>598</v>
       </c>
-      <c r="C152" s="2">
-        <v>0</v>
-      </c>
-      <c r="D152" s="2">
-        <v>0</v>
-      </c>
-      <c r="E152" s="20">
-        <v>1</v>
-      </c>
-      <c r="F152" s="20">
-        <v>1</v>
-      </c>
-      <c r="G152" s="3">
-        <v>0</v>
-      </c>
-      <c r="H152" s="18" t="s">
+      <c r="C153" s="2">
+        <v>0</v>
+      </c>
+      <c r="D153" s="2">
+        <v>0</v>
+      </c>
+      <c r="E153" s="20">
+        <v>1</v>
+      </c>
+      <c r="F153" s="20">
+        <v>1</v>
+      </c>
+      <c r="G153" s="3">
+        <v>0</v>
+      </c>
+      <c r="H153" s="18" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="18" t="s">
-        <v>593</v>
-      </c>
-      <c r="B153" s="16" t="s">
-        <v>599</v>
-      </c>
-      <c r="C153" s="2">
-        <v>0</v>
-      </c>
-      <c r="D153" s="2">
-        <v>0</v>
-      </c>
-      <c r="E153" s="20">
-        <v>1</v>
-      </c>
-      <c r="F153" s="20">
-        <v>1</v>
-      </c>
-      <c r="G153" s="3">
-        <v>0</v>
-      </c>
-      <c r="H153" s="18" t="s">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="17" t="s">
         <v>609</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A154" s="17" t="s">
-        <v>610</v>
       </c>
       <c r="B154" s="14" t="s">
         <v>122</v>
@@ -6400,475 +6400,475 @@
         <v>286</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="B155" s="23" t="s">
+        <v>531</v>
+      </c>
+      <c r="C155" s="2">
+        <v>0</v>
+      </c>
+      <c r="D155" s="2">
+        <v>0</v>
+      </c>
+      <c r="E155" s="4">
+        <v>1</v>
+      </c>
+      <c r="F155" s="22">
+        <v>1</v>
+      </c>
+      <c r="G155" s="3">
+        <v>0</v>
+      </c>
+      <c r="H155" s="17" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="B155" s="23" t="s">
+      <c r="B156" s="23" t="s">
         <v>532</v>
       </c>
-      <c r="C155" s="2">
-        <v>0</v>
-      </c>
-      <c r="D155" s="2">
-        <v>0</v>
-      </c>
-      <c r="E155" s="4">
-        <v>1</v>
-      </c>
-      <c r="F155" s="22">
-        <v>1</v>
-      </c>
-      <c r="G155" s="3">
-        <v>0</v>
-      </c>
-      <c r="H155" s="17" t="s">
+      <c r="C156" s="2">
+        <v>0</v>
+      </c>
+      <c r="D156" s="2">
+        <v>0</v>
+      </c>
+      <c r="E156" s="4">
+        <v>1</v>
+      </c>
+      <c r="F156" s="22">
+        <v>1</v>
+      </c>
+      <c r="G156" s="3">
+        <v>0</v>
+      </c>
+      <c r="H156" s="17" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A156" s="17" t="s">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="B156" s="23" t="s">
+      <c r="B157" s="23" t="s">
+        <v>538</v>
+      </c>
+      <c r="C157" s="2">
+        <v>0</v>
+      </c>
+      <c r="D157" s="2">
+        <v>0</v>
+      </c>
+      <c r="E157" s="4">
+        <v>1</v>
+      </c>
+      <c r="F157" s="22">
+        <v>1</v>
+      </c>
+      <c r="G157" s="3">
+        <v>0</v>
+      </c>
+      <c r="H157" s="17" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="17" t="s">
+        <v>572</v>
+      </c>
+      <c r="B158" s="23" t="s">
         <v>533</v>
       </c>
-      <c r="C156" s="2">
-        <v>0</v>
-      </c>
-      <c r="D156" s="2">
-        <v>0</v>
-      </c>
-      <c r="E156" s="4">
-        <v>1</v>
-      </c>
-      <c r="F156" s="22">
-        <v>1</v>
-      </c>
-      <c r="G156" s="3">
-        <v>0</v>
-      </c>
-      <c r="H156" s="17" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A157" s="17" t="s">
-        <v>572</v>
-      </c>
-      <c r="B157" s="23" t="s">
+      <c r="C158" s="2">
+        <v>0</v>
+      </c>
+      <c r="D158" s="2">
+        <v>0</v>
+      </c>
+      <c r="E158" s="4">
+        <v>1</v>
+      </c>
+      <c r="F158" s="22">
+        <v>1</v>
+      </c>
+      <c r="G158" s="3">
+        <v>0</v>
+      </c>
+      <c r="H158" s="17" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="B159" s="23" t="s">
         <v>539</v>
       </c>
-      <c r="C157" s="2">
-        <v>0</v>
-      </c>
-      <c r="D157" s="2">
-        <v>0</v>
-      </c>
-      <c r="E157" s="4">
-        <v>1</v>
-      </c>
-      <c r="F157" s="22">
-        <v>1</v>
-      </c>
-      <c r="G157" s="3">
-        <v>0</v>
-      </c>
-      <c r="H157" s="17" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A158" s="17" t="s">
-        <v>573</v>
-      </c>
-      <c r="B158" s="23" t="s">
+      <c r="C159" s="2">
+        <v>0</v>
+      </c>
+      <c r="D159" s="2">
+        <v>0</v>
+      </c>
+      <c r="E159" s="4">
+        <v>1</v>
+      </c>
+      <c r="F159" s="22">
+        <v>1</v>
+      </c>
+      <c r="G159" s="3">
+        <v>0</v>
+      </c>
+      <c r="H159" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="B160" s="23" t="s">
+        <v>540</v>
+      </c>
+      <c r="C160" s="2">
+        <v>0</v>
+      </c>
+      <c r="D160" s="2">
+        <v>0</v>
+      </c>
+      <c r="E160" s="4">
+        <v>1</v>
+      </c>
+      <c r="F160" s="22">
+        <v>1</v>
+      </c>
+      <c r="G160" s="3">
+        <v>0</v>
+      </c>
+      <c r="H160" s="17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="B161" s="23" t="s">
         <v>534</v>
       </c>
-      <c r="C158" s="2">
-        <v>0</v>
-      </c>
-      <c r="D158" s="2">
-        <v>0</v>
-      </c>
-      <c r="E158" s="4">
-        <v>1</v>
-      </c>
-      <c r="F158" s="22">
-        <v>1</v>
-      </c>
-      <c r="G158" s="3">
-        <v>0</v>
-      </c>
-      <c r="H158" s="17" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A159" s="17" t="s">
-        <v>574</v>
-      </c>
-      <c r="B159" s="23" t="s">
-        <v>540</v>
-      </c>
-      <c r="C159" s="2">
-        <v>0</v>
-      </c>
-      <c r="D159" s="2">
-        <v>0</v>
-      </c>
-      <c r="E159" s="4">
-        <v>1</v>
-      </c>
-      <c r="F159" s="22">
-        <v>1</v>
-      </c>
-      <c r="G159" s="3">
-        <v>0</v>
-      </c>
-      <c r="H159" s="17" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A160" s="17" t="s">
-        <v>575</v>
-      </c>
-      <c r="B160" s="23" t="s">
+      <c r="C161" s="2">
+        <v>0</v>
+      </c>
+      <c r="D161" s="2">
+        <v>0</v>
+      </c>
+      <c r="E161" s="4">
+        <v>1</v>
+      </c>
+      <c r="F161" s="22">
+        <v>1</v>
+      </c>
+      <c r="G161" s="3">
+        <v>0</v>
+      </c>
+      <c r="H161" s="17" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="B162" s="23" t="s">
         <v>541</v>
       </c>
-      <c r="C160" s="2">
-        <v>0</v>
-      </c>
-      <c r="D160" s="2">
-        <v>0</v>
-      </c>
-      <c r="E160" s="4">
-        <v>1</v>
-      </c>
-      <c r="F160" s="22">
-        <v>1</v>
-      </c>
-      <c r="G160" s="3">
-        <v>0</v>
-      </c>
-      <c r="H160" s="17" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A161" s="17" t="s">
-        <v>576</v>
-      </c>
-      <c r="B161" s="23" t="s">
+      <c r="C162" s="2">
+        <v>0</v>
+      </c>
+      <c r="D162" s="2">
+        <v>0</v>
+      </c>
+      <c r="E162" s="4">
+        <v>1</v>
+      </c>
+      <c r="F162" s="22">
+        <v>1</v>
+      </c>
+      <c r="G162" s="3">
+        <v>0</v>
+      </c>
+      <c r="H162" s="17" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" s="17" t="s">
+        <v>577</v>
+      </c>
+      <c r="B163" s="23" t="s">
         <v>535</v>
       </c>
-      <c r="C161" s="2">
-        <v>0</v>
-      </c>
-      <c r="D161" s="2">
-        <v>0</v>
-      </c>
-      <c r="E161" s="4">
-        <v>1</v>
-      </c>
-      <c r="F161" s="22">
-        <v>1</v>
-      </c>
-      <c r="G161" s="3">
-        <v>0</v>
-      </c>
-      <c r="H161" s="17" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A162" s="17" t="s">
-        <v>577</v>
-      </c>
-      <c r="B162" s="23" t="s">
+      <c r="C163" s="2">
+        <v>0</v>
+      </c>
+      <c r="D163" s="2">
+        <v>0</v>
+      </c>
+      <c r="E163" s="4">
+        <v>1</v>
+      </c>
+      <c r="F163" s="22">
+        <v>1</v>
+      </c>
+      <c r="G163" s="3">
+        <v>0</v>
+      </c>
+      <c r="H163" s="17" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="B164" s="23" t="s">
         <v>542</v>
       </c>
-      <c r="C162" s="2">
-        <v>0</v>
-      </c>
-      <c r="D162" s="2">
-        <v>0</v>
-      </c>
-      <c r="E162" s="4">
-        <v>1</v>
-      </c>
-      <c r="F162" s="22">
-        <v>1</v>
-      </c>
-      <c r="G162" s="3">
-        <v>0</v>
-      </c>
-      <c r="H162" s="17" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A163" s="17" t="s">
-        <v>578</v>
-      </c>
-      <c r="B163" s="23" t="s">
+      <c r="C164" s="2">
+        <v>0</v>
+      </c>
+      <c r="D164" s="2">
+        <v>0</v>
+      </c>
+      <c r="E164" s="4">
+        <v>1</v>
+      </c>
+      <c r="F164" s="22">
+        <v>1</v>
+      </c>
+      <c r="G164" s="3">
+        <v>0</v>
+      </c>
+      <c r="H164" s="17" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="B165" s="23" t="s">
+        <v>543</v>
+      </c>
+      <c r="C165" s="2">
+        <v>0</v>
+      </c>
+      <c r="D165" s="2">
+        <v>0</v>
+      </c>
+      <c r="E165" s="4">
+        <v>1</v>
+      </c>
+      <c r="F165" s="22">
+        <v>1</v>
+      </c>
+      <c r="G165" s="3">
+        <v>0</v>
+      </c>
+      <c r="H165" s="17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="B166" s="23" t="s">
+        <v>544</v>
+      </c>
+      <c r="C166" s="2">
+        <v>0</v>
+      </c>
+      <c r="D166" s="2">
+        <v>0</v>
+      </c>
+      <c r="E166" s="4">
+        <v>1</v>
+      </c>
+      <c r="F166" s="22">
+        <v>1</v>
+      </c>
+      <c r="G166" s="3">
+        <v>0</v>
+      </c>
+      <c r="H166" s="17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="B167" s="23" t="s">
         <v>536</v>
       </c>
-      <c r="C163" s="2">
-        <v>0</v>
-      </c>
-      <c r="D163" s="2">
-        <v>0</v>
-      </c>
-      <c r="E163" s="4">
-        <v>1</v>
-      </c>
-      <c r="F163" s="22">
-        <v>1</v>
-      </c>
-      <c r="G163" s="3">
-        <v>0</v>
-      </c>
-      <c r="H163" s="17" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A164" s="17" t="s">
-        <v>579</v>
-      </c>
-      <c r="B164" s="23" t="s">
-        <v>543</v>
-      </c>
-      <c r="C164" s="2">
-        <v>0</v>
-      </c>
-      <c r="D164" s="2">
-        <v>0</v>
-      </c>
-      <c r="E164" s="4">
-        <v>1</v>
-      </c>
-      <c r="F164" s="22">
-        <v>1</v>
-      </c>
-      <c r="G164" s="3">
-        <v>0</v>
-      </c>
-      <c r="H164" s="17" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A165" s="17" t="s">
-        <v>580</v>
-      </c>
-      <c r="B165" s="23" t="s">
-        <v>544</v>
-      </c>
-      <c r="C165" s="2">
-        <v>0</v>
-      </c>
-      <c r="D165" s="2">
-        <v>0</v>
-      </c>
-      <c r="E165" s="4">
-        <v>1</v>
-      </c>
-      <c r="F165" s="22">
-        <v>1</v>
-      </c>
-      <c r="G165" s="3">
-        <v>0</v>
-      </c>
-      <c r="H165" s="17" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A166" s="17" t="s">
-        <v>581</v>
-      </c>
-      <c r="B166" s="23" t="s">
+      <c r="C167" s="2">
+        <v>0</v>
+      </c>
+      <c r="D167" s="2">
+        <v>0</v>
+      </c>
+      <c r="E167" s="4">
+        <v>1</v>
+      </c>
+      <c r="F167" s="22">
+        <v>1</v>
+      </c>
+      <c r="G167" s="3">
+        <v>0</v>
+      </c>
+      <c r="H167" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="B168" s="23" t="s">
         <v>545</v>
       </c>
-      <c r="C166" s="2">
-        <v>0</v>
-      </c>
-      <c r="D166" s="2">
-        <v>0</v>
-      </c>
-      <c r="E166" s="4">
-        <v>1</v>
-      </c>
-      <c r="F166" s="22">
-        <v>1</v>
-      </c>
-      <c r="G166" s="3">
-        <v>0</v>
-      </c>
-      <c r="H166" s="17" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A167" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="B167" s="23" t="s">
+      <c r="C168" s="2">
+        <v>0</v>
+      </c>
+      <c r="D168" s="2">
+        <v>0</v>
+      </c>
+      <c r="E168" s="4">
+        <v>1</v>
+      </c>
+      <c r="F168" s="22">
+        <v>1</v>
+      </c>
+      <c r="G168" s="3">
+        <v>0</v>
+      </c>
+      <c r="H168" s="17" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" s="17" t="s">
+        <v>583</v>
+      </c>
+      <c r="B169" s="23" t="s">
         <v>537</v>
       </c>
-      <c r="C167" s="2">
-        <v>0</v>
-      </c>
-      <c r="D167" s="2">
-        <v>0</v>
-      </c>
-      <c r="E167" s="4">
-        <v>1</v>
-      </c>
-      <c r="F167" s="22">
-        <v>1</v>
-      </c>
-      <c r="G167" s="3">
-        <v>0</v>
-      </c>
-      <c r="H167" s="17" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A168" s="17" t="s">
-        <v>583</v>
-      </c>
-      <c r="B168" s="23" t="s">
+      <c r="C169" s="2">
+        <v>0</v>
+      </c>
+      <c r="D169" s="2">
+        <v>0</v>
+      </c>
+      <c r="E169" s="4">
+        <v>1</v>
+      </c>
+      <c r="F169" s="22">
+        <v>1</v>
+      </c>
+      <c r="G169" s="3">
+        <v>0</v>
+      </c>
+      <c r="H169" s="17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="B170" s="23" t="s">
         <v>546</v>
       </c>
-      <c r="C168" s="2">
-        <v>0</v>
-      </c>
-      <c r="D168" s="2">
-        <v>0</v>
-      </c>
-      <c r="E168" s="4">
-        <v>1</v>
-      </c>
-      <c r="F168" s="22">
-        <v>1</v>
-      </c>
-      <c r="G168" s="3">
-        <v>0</v>
-      </c>
-      <c r="H168" s="17" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A169" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="B169" s="23" t="s">
-        <v>538</v>
-      </c>
-      <c r="C169" s="2">
-        <v>0</v>
-      </c>
-      <c r="D169" s="2">
-        <v>0</v>
-      </c>
-      <c r="E169" s="4">
-        <v>1</v>
-      </c>
-      <c r="F169" s="22">
-        <v>1</v>
-      </c>
-      <c r="G169" s="3">
-        <v>0</v>
-      </c>
-      <c r="H169" s="17" t="s">
+      <c r="C170" s="2">
+        <v>0</v>
+      </c>
+      <c r="D170" s="2">
+        <v>0</v>
+      </c>
+      <c r="E170" s="4">
+        <v>1</v>
+      </c>
+      <c r="F170" s="22">
+        <v>1</v>
+      </c>
+      <c r="G170" s="3">
+        <v>0</v>
+      </c>
+      <c r="H170" s="17" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A170" s="17" t="s">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="B170" s="23" t="s">
+      <c r="B171" s="23" t="s">
+        <v>548</v>
+      </c>
+      <c r="C171" s="2">
+        <v>0</v>
+      </c>
+      <c r="D171" s="2">
+        <v>0</v>
+      </c>
+      <c r="E171" s="4">
+        <v>1</v>
+      </c>
+      <c r="F171" s="22">
+        <v>1</v>
+      </c>
+      <c r="G171" s="3">
+        <v>0</v>
+      </c>
+      <c r="H171" s="17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="B172" s="23" t="s">
         <v>547</v>
       </c>
-      <c r="C170" s="2">
-        <v>0</v>
-      </c>
-      <c r="D170" s="2">
-        <v>0</v>
-      </c>
-      <c r="E170" s="4">
-        <v>1</v>
-      </c>
-      <c r="F170" s="22">
-        <v>1</v>
-      </c>
-      <c r="G170" s="3">
-        <v>0</v>
-      </c>
-      <c r="H170" s="17" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A171" s="17" t="s">
-        <v>586</v>
-      </c>
-      <c r="B171" s="23" t="s">
-        <v>549</v>
-      </c>
-      <c r="C171" s="2">
-        <v>0</v>
-      </c>
-      <c r="D171" s="2">
-        <v>0</v>
-      </c>
-      <c r="E171" s="4">
-        <v>1</v>
-      </c>
-      <c r="F171" s="22">
-        <v>1</v>
-      </c>
-      <c r="G171" s="3">
-        <v>0</v>
-      </c>
-      <c r="H171" s="17" t="s">
+      <c r="C172" s="2">
+        <v>0</v>
+      </c>
+      <c r="D172" s="2">
+        <v>0</v>
+      </c>
+      <c r="E172" s="4">
+        <v>1</v>
+      </c>
+      <c r="F172" s="22">
+        <v>1</v>
+      </c>
+      <c r="G172" s="3">
+        <v>0</v>
+      </c>
+      <c r="H172" s="17" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A172" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="B172" s="23" t="s">
-        <v>548</v>
-      </c>
-      <c r="C172" s="2">
-        <v>0</v>
-      </c>
-      <c r="D172" s="2">
-        <v>0</v>
-      </c>
-      <c r="E172" s="4">
-        <v>1</v>
-      </c>
-      <c r="F172" s="22">
-        <v>1</v>
-      </c>
-      <c r="G172" s="3">
-        <v>0</v>
-      </c>
-      <c r="H172" s="17" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
         <v>443</v>
       </c>
@@ -6894,9 +6894,9 @@
         <v>287</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B174" s="14" t="s">
         <v>124</v>
@@ -6920,7 +6920,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
         <v>444</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
         <v>445</v>
       </c>
@@ -6972,59 +6972,59 @@
         <v>290</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="B177" s="14" t="s">
         <v>564</v>
       </c>
-      <c r="B177" s="14" t="s">
+      <c r="C177" s="2">
+        <v>0</v>
+      </c>
+      <c r="D177" s="2">
+        <v>0</v>
+      </c>
+      <c r="E177" s="20">
+        <v>1</v>
+      </c>
+      <c r="F177" s="22">
+        <v>1</v>
+      </c>
+      <c r="G177" s="3">
+        <v>1</v>
+      </c>
+      <c r="H177" s="17" t="s">
         <v>565</v>
       </c>
-      <c r="C177" s="2">
-        <v>0</v>
-      </c>
-      <c r="D177" s="2">
-        <v>0</v>
-      </c>
-      <c r="E177" s="20">
-        <v>1</v>
-      </c>
-      <c r="F177" s="22">
-        <v>1</v>
-      </c>
-      <c r="G177" s="3">
-        <v>1</v>
-      </c>
-      <c r="H177" s="17" t="s">
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="17" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A178" s="17" t="s">
+      <c r="B178" s="14" t="s">
         <v>567</v>
       </c>
-      <c r="B178" s="14" t="s">
+      <c r="C178" s="2">
+        <v>0</v>
+      </c>
+      <c r="D178" s="2">
+        <v>0</v>
+      </c>
+      <c r="E178" s="20">
+        <v>1</v>
+      </c>
+      <c r="F178" s="22">
+        <v>1</v>
+      </c>
+      <c r="G178" s="3">
+        <v>1</v>
+      </c>
+      <c r="H178" s="17" t="s">
         <v>568</v>
       </c>
-      <c r="C178" s="2">
-        <v>0</v>
-      </c>
-      <c r="D178" s="2">
-        <v>0</v>
-      </c>
-      <c r="E178" s="20">
-        <v>1</v>
-      </c>
-      <c r="F178" s="22">
-        <v>1</v>
-      </c>
-      <c r="G178" s="3">
-        <v>1</v>
-      </c>
-      <c r="H178" s="17" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
         <v>446</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
         <v>447</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
         <v>448</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
         <v>449</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
         <v>450</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
         <v>451</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
         <v>452</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
         <v>453</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
         <v>454</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
         <v>455</v>
       </c>
@@ -7284,7 +7284,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
         <v>456</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
         <v>457</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
         <v>458</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
         <v>459</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
         <v>460</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
         <v>461</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
         <v>462</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="17" t="s">
         <v>463</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="17" t="s">
         <v>464</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="17" t="s">
         <v>465</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="17" t="s">
         <v>466</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="17" t="s">
         <v>467</v>
       </c>
@@ -7596,7 +7596,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="17" t="s">
         <v>468</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="17" t="s">
         <v>469</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="17" t="s">
         <v>470</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="17" t="s">
         <v>471</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="17" t="s">
         <v>472</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="17" t="s">
         <v>473</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="17" t="s">
         <v>474</v>
       </c>
@@ -7778,9 +7778,9 @@
         <v>319</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="17" t="s">
-        <v>475</v>
+        <v>643</v>
       </c>
       <c r="B208" s="14" t="s">
         <v>156</v>
@@ -7804,9 +7804,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B209" s="14" t="s">
         <v>157</v>
@@ -7830,9 +7830,9 @@
         <v>321</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B210" s="14" t="s">
         <v>158</v>
@@ -7856,9 +7856,9 @@
         <v>322</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B211" s="14" t="s">
         <v>159</v>
@@ -7882,9 +7882,9 @@
         <v>323</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B212" s="14" t="s">
         <v>160</v>
@@ -7908,9 +7908,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B213" s="14" t="s">
         <v>161</v>
@@ -7934,9 +7934,9 @@
         <v>325</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B214" s="16" t="s">
         <v>162</v>
@@ -7960,9 +7960,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B215" s="16" t="s">
         <v>163</v>
@@ -7986,9 +7986,9 @@
         <v>327</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B216" s="16" t="s">
         <v>164</v>
@@ -8012,9 +8012,9 @@
         <v>328</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="18" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B217" s="16" t="s">
         <v>165</v>
@@ -8038,9 +8038,9 @@
         <v>329</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B218" s="16" t="s">
         <v>166</v>
@@ -8064,9 +8064,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="18" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B219" s="16" t="s">
         <v>167</v>
@@ -8090,9 +8090,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="18" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B220" s="16" t="s">
         <v>168</v>
@@ -8116,9 +8116,9 @@
         <v>213</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B221" s="16" t="s">
         <v>169</v>
@@ -8142,30 +8142,30 @@
         <v>212</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="B222" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="B222" s="5" t="s">
+      <c r="C222" s="2">
+        <v>1</v>
+      </c>
+      <c r="D222" s="2">
+        <v>1</v>
+      </c>
+      <c r="E222" s="4">
+        <v>1</v>
+      </c>
+      <c r="F222" s="3">
+        <v>1</v>
+      </c>
+      <c r="G222" s="3">
+        <v>0</v>
+      </c>
+      <c r="H222" s="5" t="s">
         <v>642</v>
-      </c>
-      <c r="C222" s="2">
-        <v>1</v>
-      </c>
-      <c r="D222" s="2">
-        <v>1</v>
-      </c>
-      <c r="E222" s="4">
-        <v>1</v>
-      </c>
-      <c r="F222" s="3">
-        <v>1</v>
-      </c>
-      <c r="G222" s="3">
-        <v>0</v>
-      </c>
-      <c r="H222" s="5" t="s">
-        <v>643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various updates (also memory optimisation)
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_india.xlsx
+++ b/inst/extdata/main_dict_india.xlsx
@@ -2027,22 +2027,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
     <col min="5" max="5" width="9.25" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="3"/>
-    <col min="8" max="8" width="31.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>431</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>493</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>457</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>491</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>467</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>492</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>474</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>476</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>478</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>480</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>482</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>484</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>294</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>295</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>432</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>296</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>297</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>437</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>298</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>299</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>300</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>436</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>302</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>303</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>304</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>301</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>305</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>306</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>307</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>308</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>309</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>310</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>311</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>312</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>313</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>314</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>315</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>449</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>453</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>316</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>317</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>318</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>319</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>320</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>321</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>322</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>323</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>324</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>325</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>326</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>521</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>524</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>327</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>328</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>330</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>331</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>329</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>471</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>472</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>468</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>469</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>488</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>470</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>440</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>332</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>333</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>445</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
         <v>447</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>473</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>499</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>501</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
         <v>334</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
         <v>335</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
         <v>336</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
         <v>337</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
         <v>517</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
         <v>338</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
         <v>339</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
         <v>340</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
         <v>341</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
         <v>342</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
         <v>343</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
         <v>344</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
         <v>345</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
         <v>346</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
         <v>347</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
         <v>348</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
         <v>349</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
         <v>350</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
         <v>351</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
         <v>352</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="14" t="s">
         <v>353</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
         <v>354</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
         <v>355</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="14" t="s">
         <v>356</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="14" t="s">
         <v>357</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="14" t="s">
         <v>358</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="14" t="s">
         <v>359</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="14" t="s">
         <v>360</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="14" t="s">
         <v>361</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="14" t="s">
         <v>362</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="14" t="s">
         <v>363</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="14" t="s">
         <v>364</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
         <v>365</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
         <v>366</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
         <v>367</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
         <v>368</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
         <v>369</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
         <v>370</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
         <v>371</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
         <v>372</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="14" t="s">
         <v>373</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="14" t="s">
         <v>374</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="14" t="s">
         <v>375</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="14" t="s">
         <v>376</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="14" t="s">
         <v>377</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="14" t="s">
         <v>378</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="14" t="s">
         <v>379</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="14" t="s">
         <v>380</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="14" t="s">
         <v>381</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="14" t="s">
         <v>382</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="14" t="s">
         <v>383</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="14" t="s">
         <v>384</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="14" t="s">
         <v>385</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="14" t="s">
         <v>505</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="14" t="s">
         <v>386</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="14" t="s">
         <v>507</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
         <v>509</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
         <v>514</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
         <v>387</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
         <v>456</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
         <v>388</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
         <v>389</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
         <v>460</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
         <v>463</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
         <v>390</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
         <v>391</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
         <v>392</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
         <v>393</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
         <v>394</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
         <v>395</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
         <v>396</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
         <v>397</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
         <v>398</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
         <v>399</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
         <v>400</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
         <v>401</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
         <v>402</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
         <v>504</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="14" t="s">
         <v>403</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="14" t="s">
         <v>404</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="14" t="s">
         <v>405</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="14" t="s">
         <v>406</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="14" t="s">
         <v>407</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="14" t="s">
         <v>408</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="14" t="s">
         <v>409</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="14" t="s">
         <v>410</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="14" t="s">
         <v>411</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="14" t="s">
         <v>412</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="14" t="s">
         <v>413</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="14" t="s">
         <v>414</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="14" t="s">
         <v>415</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="14" t="s">
         <v>416</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="14" t="s">
         <v>417</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="14" t="s">
         <v>498</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="14" t="s">
         <v>418</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="14" t="s">
         <v>419</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="14" t="s">
         <v>420</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="14" t="s">
         <v>421</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="14" t="s">
         <v>422</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="15" t="s">
         <v>423</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="15" t="s">
         <v>424</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="15" t="s">
         <v>425</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="15" t="s">
         <v>426</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="15" t="s">
         <v>427</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="15" t="s">
         <v>428</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="15" t="s">
         <v>429</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="15" t="s">
         <v>430</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>495</v>
       </c>

</xml_diff>

<commit_message>
Refactoring of screening/Day 0 checks
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_india.xlsx
+++ b/inst/extdata/main_dict_india.xlsx
@@ -1424,9 +1424,6 @@
     <t>i2_1o</t>
   </si>
   <si>
-    <t>yg_infant_ctg</t>
-  </si>
-  <si>
     <t>end</t>
   </si>
   <si>
@@ -1605,6 +1602,9 @@
   </si>
   <si>
     <t>child_id_manual</t>
+  </si>
+  <si>
+    <t>who_age_ctg</t>
   </si>
 </sst>
 </file>
@@ -2027,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD60"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2174,11 +2174,11 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>494</v>
-      </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2226,10 +2226,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -2252,10 +2252,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2273,15 +2273,15 @@
         <v>0</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -2299,16 +2299,16 @@
         <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>475</v>
-      </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
@@ -2325,16 +2325,16 @@
         <v>1</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
+        <v>475</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>477</v>
-      </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
@@ -2351,16 +2351,16 @@
         <v>1</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>478</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>479</v>
-      </c>
       <c r="C13" s="2">
         <v>1</v>
       </c>
@@ -2377,16 +2377,16 @@
         <v>1</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>481</v>
-      </c>
       <c r="C14" s="2">
         <v>1</v>
       </c>
@@ -2403,16 +2403,16 @@
         <v>1</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>483</v>
-      </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
@@ -2429,16 +2429,16 @@
         <v>1</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>484</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>485</v>
-      </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2801,7 +2801,7 @@
         <v>301</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>466</v>
+        <v>526</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -3448,54 +3448,54 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <v>1</v>
+      </c>
+      <c r="H55" s="6" t="s">
         <v>522</v>
-      </c>
-      <c r="C55" s="2">
-        <v>1</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4">
-        <v>1</v>
-      </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
-      <c r="G55" s="3">
-        <v>1</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="4">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3">
+        <v>1</v>
+      </c>
+      <c r="H56" s="6" t="s">
         <v>524</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="C56" s="2">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4">
-        <v>1</v>
-      </c>
-      <c r="F56" s="3">
-        <v>1</v>
-      </c>
-      <c r="G56" s="3">
-        <v>1</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -3630,7 +3630,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>32</v>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>33</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>38</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>39</v>
@@ -3734,33 +3734,33 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="B66" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="C66" s="2">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="4">
+        <v>0</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3">
+        <v>0</v>
+      </c>
+      <c r="H66" s="9" t="s">
         <v>489</v>
-      </c>
-      <c r="C66" s="2">
-        <v>0</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="4">
-        <v>0</v>
-      </c>
-      <c r="F66" s="4">
-        <v>0</v>
-      </c>
-      <c r="G66" s="3">
-        <v>0</v>
-      </c>
-      <c r="H66" s="9" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>434</v>
@@ -3916,7 +3916,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>444</v>
@@ -3942,10 +3942,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="B74" s="11" t="s">
         <v>499</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>500</v>
       </c>
       <c r="C74" s="2">
         <v>1</v>
@@ -3968,10 +3968,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>501</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>502</v>
       </c>
       <c r="C75" s="2">
         <v>1</v>
@@ -4098,11 +4098,11 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="B80" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="B80" s="13" t="s">
-        <v>518</v>
-      </c>
       <c r="C80" s="2">
         <v>0</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -5372,7 +5372,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B129" s="14" t="s">
         <v>103</v>
@@ -5393,7 +5393,7 @@
         <v>0</v>
       </c>
       <c r="H129" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
@@ -5424,80 +5424,80 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="C131" s="2">
+        <v>0</v>
+      </c>
+      <c r="D131" s="2">
+        <v>0</v>
+      </c>
+      <c r="E131" s="17">
+        <v>1</v>
+      </c>
+      <c r="F131" s="19">
+        <v>1</v>
+      </c>
+      <c r="G131" s="3">
+        <v>0</v>
+      </c>
+      <c r="H131" s="14" t="s">
         <v>507</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>506</v>
-      </c>
-      <c r="C131" s="2">
-        <v>0</v>
-      </c>
-      <c r="D131" s="2">
-        <v>0</v>
-      </c>
-      <c r="E131" s="17">
-        <v>1</v>
-      </c>
-      <c r="F131" s="19">
-        <v>1</v>
-      </c>
-      <c r="G131" s="3">
-        <v>0</v>
-      </c>
-      <c r="H131" s="14" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="B132" s="14" t="s">
         <v>509</v>
       </c>
-      <c r="B132" s="14" t="s">
+      <c r="C132" s="2">
+        <v>0</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0</v>
+      </c>
+      <c r="E132" s="17">
+        <v>1</v>
+      </c>
+      <c r="F132" s="19">
+        <v>1</v>
+      </c>
+      <c r="G132" s="3">
+        <v>0</v>
+      </c>
+      <c r="H132" s="14" t="s">
         <v>510</v>
-      </c>
-      <c r="C132" s="2">
-        <v>0</v>
-      </c>
-      <c r="D132" s="2">
-        <v>0</v>
-      </c>
-      <c r="E132" s="17">
-        <v>1</v>
-      </c>
-      <c r="F132" s="19">
-        <v>1</v>
-      </c>
-      <c r="G132" s="3">
-        <v>0</v>
-      </c>
-      <c r="H132" s="14" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0</v>
+      </c>
+      <c r="D133" s="2">
+        <v>0</v>
+      </c>
+      <c r="E133" s="17">
+        <v>1</v>
+      </c>
+      <c r="F133" s="19">
+        <v>1</v>
+      </c>
+      <c r="G133" s="3">
+        <v>0</v>
+      </c>
+      <c r="H133" s="14" t="s">
         <v>514</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>513</v>
-      </c>
-      <c r="C133" s="2">
-        <v>0</v>
-      </c>
-      <c r="D133" s="2">
-        <v>0</v>
-      </c>
-      <c r="E133" s="17">
-        <v>1</v>
-      </c>
-      <c r="F133" s="19">
-        <v>1</v>
-      </c>
-      <c r="G133" s="3">
-        <v>0</v>
-      </c>
-      <c r="H133" s="14" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -5996,10 +5996,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6017,7 +6017,7 @@
         <v>0</v>
       </c>
       <c r="H153" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -6412,7 +6412,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="14" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B169" s="14" t="s">
         <v>137</v>
@@ -6433,7 +6433,7 @@
         <v>0</v>
       </c>
       <c r="H169" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
@@ -6776,28 +6776,28 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B183" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="B183" s="5" t="s">
+      <c r="C183" s="2">
+        <v>1</v>
+      </c>
+      <c r="D183" s="2">
+        <v>1</v>
+      </c>
+      <c r="E183" s="4">
+        <v>1</v>
+      </c>
+      <c r="F183" s="3">
+        <v>1</v>
+      </c>
+      <c r="G183" s="3">
+        <v>0</v>
+      </c>
+      <c r="H183" s="5" t="s">
         <v>496</v>
-      </c>
-      <c r="C183" s="2">
-        <v>1</v>
-      </c>
-      <c r="D183" s="2">
-        <v>1</v>
-      </c>
-      <c r="E183" s="4">
-        <v>1</v>
-      </c>
-      <c r="F183" s="3">
-        <v>1</v>
-      </c>
-      <c r="G183" s="3">
-        <v>0</v>
-      </c>
-      <c r="H183" s="5" t="s">
-        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Export Day 0 form version
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_india.xlsx
+++ b/inst/extdata/main_dict_india.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="529">
   <si>
     <t>old</t>
   </si>
@@ -1605,6 +1605,12 @@
   </si>
   <si>
     <t>who_age_ctg</t>
+  </si>
+  <si>
+    <t>FormVersion</t>
+  </si>
+  <si>
+    <t>form_version</t>
   </si>
 </sst>
 </file>
@@ -2025,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:H184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="I174" sqref="I174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6800,6 +6806,32 @@
         <v>496</v>
       </c>
     </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A184" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="C184" s="2">
+        <v>1</v>
+      </c>
+      <c r="D184" s="2">
+        <v>1</v>
+      </c>
+      <c r="E184" s="2">
+        <v>1</v>
+      </c>
+      <c r="F184" s="2">
+        <v>1</v>
+      </c>
+      <c r="G184" s="2">
+        <v>1</v>
+      </c>
+      <c r="H184" s="5" t="s">
+        <v>527</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId1"/>

</xml_diff>